<commit_message>
DSR update + fixing soc/DSR values
</commit_message>
<xml_diff>
--- a/Input Data/Techno-economic parameters/Generator_efficiencies.xlsx
+++ b/Input Data/Techno-economic parameters/Generator_efficiencies.xlsx
@@ -432,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +449,7 @@
     <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -481,7 +481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -515,8 +515,16 @@
         <f>C2+F2/B2+H2/B2*I2</f>
         <v>85.02181818181819</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <f>F2/B2</f>
+        <v>51.709090909090911</v>
+      </c>
+      <c r="M2">
+        <f>H2*I2/B2</f>
+        <v>31.712727272727278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -551,7 +559,7 @@
         <v>96.54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -586,7 +594,7 @@
         <v>90.465000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -621,7 +629,7 @@
         <v>14.127272727272727</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -656,7 +664,7 @@
         <v>116.30499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -691,7 +699,7 @@
         <v>114.3857142857143</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -726,7 +734,7 @@
         <v>231.23142857142858</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -761,7 +769,7 @@
         <v>264.00285714285712</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -786,7 +794,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -815,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -844,7 +852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -870,7 +878,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -899,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -928,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>

</xml_diff>